<commit_message>
Ajustes para la vista manu responsive del dashboard, ajustes para la opcion de edicion en movimientos recientes, creacion de un nuevo modal en tabla que permite elimiar los productos y editarlos
</commit_message>
<xml_diff>
--- a/data/gastos.xlsx
+++ b/data/gastos.xlsx
@@ -397,13 +397,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>fecha</v>
+      </c>
+      <c r="C1" t="str">
+        <v>descripcion</v>
+      </c>
+      <c r="D1" t="str">
+        <v>categoria</v>
+      </c>
+      <c r="E1" t="str">
+        <v>monto</v>
+      </c>
+      <c r="F1" t="str">
+        <v>responsable</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1771030088116</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-02-13</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Pago Bailarin</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E2">
+        <v>20000</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1771038851670</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-02-13</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Hielo</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="E3">
+        <v>105600</v>
+      </c>
+      <c r="F3" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1771041644127</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-02-13</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Turno jhojan</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E4">
+        <v>80000</v>
+      </c>
+      <c r="F4" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1771041670738</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-13</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve">Turno Luz Helena </v>
+      </c>
+      <c r="D5" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E5">
+        <v>80000</v>
+      </c>
+      <c r="F5" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1771041682253</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-02-13</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Turno Luisa</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E6">
+        <v>80000</v>
+      </c>
+      <c r="F6" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1771118848931</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Papel higenico</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="E7">
+        <v>14000</v>
+      </c>
+      <c r="F7" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1771134777376</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Zumo de limon</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="E8">
+        <v>30000</v>
+      </c>
+      <c r="F8" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1771134822848</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Julian</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E9">
+        <v>80000</v>
+      </c>
+      <c r="F9" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1771134832592</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Martha</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E10">
+        <v>80000</v>
+      </c>
+      <c r="F10" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1771134843141</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Valeria</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E11">
+        <v>70000</v>
+      </c>
+      <c r="F11" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>1771134850508</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Juanita</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E12">
+        <v>70000</v>
+      </c>
+      <c r="F12" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>1771134859009</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Alexander</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E13">
+        <v>70000</v>
+      </c>
+      <c r="F13" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>1771134866589</v>
+      </c>
+      <c r="B14" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Jhojan</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E14">
+        <v>70000</v>
+      </c>
+      <c r="F14" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>1771134873452</v>
+      </c>
+      <c r="B15" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Fredy</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E15">
+        <v>70000</v>
+      </c>
+      <c r="F15" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>1771134881166</v>
+      </c>
+      <c r="B16" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Laura</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E16">
+        <v>70000</v>
+      </c>
+      <c r="F16" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>1771134911552</v>
+      </c>
+      <c r="B17" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Dreisy</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E17">
+        <v>80000</v>
+      </c>
+      <c r="F17" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>1771134921425</v>
+      </c>
+      <c r="B18" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve">Juan Carlos </v>
+      </c>
+      <c r="D18" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E18">
+        <v>80000</v>
+      </c>
+      <c r="F18" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>1771134939618</v>
+      </c>
+      <c r="B19" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Sebastian</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E19">
+        <v>150000</v>
+      </c>
+      <c r="F19" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>1771134947079</v>
+      </c>
+      <c r="B20" t="str">
+        <v>2026-02-14</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Luisa</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E20">
+        <v>80000</v>
+      </c>
+      <c r="F20" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes para la vista dashboard incluye filtro de hora, nuevo Kpi producto mas vendido, se agrega scroll en inventario, se agregan categorias de cafeteria y de barra
</commit_message>
<xml_diff>
--- a/data/gastos.xlsx
+++ b/data/gastos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -802,9 +802,229 @@
         <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21">
+        <v>1771624904383</v>
+      </c>
+      <c r="B21" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Cafeteria Doña Martha</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E21">
+        <v>632240</v>
+      </c>
+      <c r="F21" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1771624963201</v>
+      </c>
+      <c r="B22" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Agua</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Servicios</v>
+      </c>
+      <c r="E22">
+        <v>432850</v>
+      </c>
+      <c r="F22" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>1771632832729</v>
+      </c>
+      <c r="B23" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Compras</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E23">
+        <v>2224290</v>
+      </c>
+      <c r="F23" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>1771633930022</v>
+      </c>
+      <c r="B24" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Zumo de limon</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E24">
+        <v>40000</v>
+      </c>
+      <c r="F24" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1771633942158</v>
+      </c>
+      <c r="B25" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Martin</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E25">
+        <v>50000</v>
+      </c>
+      <c r="F25" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>1771639250275</v>
+      </c>
+      <c r="B26" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Bailarin</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E26">
+        <v>20000</v>
+      </c>
+      <c r="F26" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>1771639250285</v>
+      </c>
+      <c r="B27" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Bailarin</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E27">
+        <v>20000</v>
+      </c>
+      <c r="F27" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>1771641168472</v>
+      </c>
+      <c r="B28" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Hielo</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E28">
+        <v>84000</v>
+      </c>
+      <c r="F28" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>1771644118288</v>
+      </c>
+      <c r="B29" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Luz Helena</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E29">
+        <v>80000</v>
+      </c>
+      <c r="F29" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>1771644127448</v>
+      </c>
+      <c r="B30" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Fredy</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E30">
+        <v>80000</v>
+      </c>
+      <c r="F30" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>1771644141358</v>
+      </c>
+      <c r="B31" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C31" t="str">
+        <v xml:space="preserve">Luisa </v>
+      </c>
+      <c r="D31" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E31">
+        <v>80000</v>
+      </c>
+      <c r="F31" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se carga de manera masiva ventas del mes de enero, se actualiza la vista gastos con la inclusion de filtros y creacion de la categoria cafeteria
</commit_message>
<xml_diff>
--- a/data/gastos.xlsx
+++ b/data/gastos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1022,9 +1022,389 @@
         <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32">
+        <v>1771743882115</v>
+      </c>
+      <c r="B32" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Martha</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E32">
+        <v>80000</v>
+      </c>
+      <c r="F32" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>1771743914552</v>
+      </c>
+      <c r="B33" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Dreisy</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E33">
+        <v>80000</v>
+      </c>
+      <c r="F33" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>1771743947518</v>
+      </c>
+      <c r="B34" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Luisa vallejo</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E34">
+        <v>80000</v>
+      </c>
+      <c r="F34" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>1771743955114</v>
+      </c>
+      <c r="B35" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Julian</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E35">
+        <v>80000</v>
+      </c>
+      <c r="F35" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>1771743971143</v>
+      </c>
+      <c r="B36" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Alexander</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E36">
+        <v>70000</v>
+      </c>
+      <c r="F36" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>1771744008831</v>
+      </c>
+      <c r="B37" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Juanita</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E37">
+        <v>70000</v>
+      </c>
+      <c r="F37" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>1771744022489</v>
+      </c>
+      <c r="B38" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Valeria</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E38">
+        <v>70000</v>
+      </c>
+      <c r="F38" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>1771744045848</v>
+      </c>
+      <c r="B39" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Jhojan</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E39">
+        <v>70000</v>
+      </c>
+      <c r="F39" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>1771744059511</v>
+      </c>
+      <c r="B40" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Sebastian</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E40">
+        <v>150000</v>
+      </c>
+      <c r="F40" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>1771744073710</v>
+      </c>
+      <c r="B41" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Juan Carlos</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E41">
+        <v>80000</v>
+      </c>
+      <c r="F41" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>1771744099156</v>
+      </c>
+      <c r="B42" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Laura</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E42">
+        <v>70000</v>
+      </c>
+      <c r="F42" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1771744302410</v>
+      </c>
+      <c r="B43" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Papel, trapos, cloro</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E43">
+        <v>42370</v>
+      </c>
+      <c r="F43" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>1772230354842</v>
+      </c>
+      <c r="B44" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Energia</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Servicios</v>
+      </c>
+      <c r="E44">
+        <v>723540</v>
+      </c>
+      <c r="F44" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>1772230494337</v>
+      </c>
+      <c r="B45" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Prestamo Mr Tango- Sayci-Acinpro</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="E45">
+        <v>5800000</v>
+      </c>
+      <c r="F45" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>1772234485905</v>
+      </c>
+      <c r="B46" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Zumo de limon</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Insumos</v>
+      </c>
+      <c r="E46">
+        <v>40000</v>
+      </c>
+      <c r="F46" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>1772246917060</v>
+      </c>
+      <c r="B47" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Jhojan Buitrago</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E47">
+        <v>80000</v>
+      </c>
+      <c r="F47" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>1772246944016</v>
+      </c>
+      <c r="B48" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Fredy Ramirez</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E48">
+        <v>80000</v>
+      </c>
+      <c r="F48" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>1772247070113</v>
+      </c>
+      <c r="B49" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C49" t="str">
+        <v xml:space="preserve">Sebastian </v>
+      </c>
+      <c r="D49" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E49">
+        <v>80000</v>
+      </c>
+      <c r="F49" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>1772247096948</v>
+      </c>
+      <c r="B50" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Luisa Vallejo</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Nomina</v>
+      </c>
+      <c r="E50">
+        <v>80000</v>
+      </c>
+      <c r="F50" t="str">
+        <v>{"nombre":"Luisa","rol":"ADMIN"}</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>